<commit_message>
added upload only endpoint
</commit_message>
<xml_diff>
--- a/acibootstrap/files/vars/ACI-Bootstrap-Tool.xlsx
+++ b/acibootstrap/files/vars/ACI-Bootstrap-Tool.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="105">
   <si>
     <t/>
   </si>
@@ -234,7 +234,7 @@
     <t>chapeter</t>
   </si>
   <si>
-    <t>test customer</t>
+    <t>demo-customer</t>
   </si>
   <si>
     <t>10.94.238.5</t>
@@ -261,63 +261,63 @@
     <t>208.67.220.220</t>
   </si>
   <si>
-    <t>10G-auto</t>
+    <t>1G-auto</t>
   </si>
   <si>
     <t>10.94.238.150</t>
   </si>
   <si>
-    <t>10.94.238.200</t>
+    <t>10.94.238.160</t>
   </si>
   <si>
     <t>10.94.238.1/24</t>
   </si>
   <si>
-    <t>10.94.238.50</t>
-  </si>
-  <si>
-    <t>pov</t>
+    <t>10.94.238.58</t>
+  </si>
+  <si>
+    <t>demo-dc</t>
   </si>
   <si>
     <t>administrator@vsphere.local</t>
   </si>
   <si>
-    <t>cisco</t>
-  </si>
-  <si>
-    <t>tenant-1</t>
+    <t>C!sco123</t>
+  </si>
+  <si>
+    <t>POV-3tier-L3_1</t>
   </si>
   <si>
     <t>external</t>
   </si>
   <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>172.16.32.1/24</t>
+  </si>
+  <si>
+    <t>172.16.33.1/24</t>
+  </si>
+  <si>
+    <t>172.16.34.1/24</t>
+  </si>
+  <si>
+    <t>ospf</t>
+  </si>
+  <si>
+    <t>nssa</t>
+  </si>
+  <si>
+    <t>10.1.1.1/30</t>
+  </si>
+  <si>
+    <t>10.1.2.1/30</t>
+  </si>
+  <si>
     <t>1.1.1.1/24</t>
   </si>
   <si>
-    <t>2.2.2.2/24</t>
-  </si>
-  <si>
-    <t>private</t>
-  </si>
-  <si>
-    <t>3.3.3.3/24</t>
-  </si>
-  <si>
-    <t>ospf</t>
-  </si>
-  <si>
-    <t>nssa</t>
-  </si>
-  <si>
-    <t>10.1.1.1/30</t>
-  </si>
-  <si>
-    <t>10.1.2.1/30</t>
-  </si>
-  <si>
-    <t>tenant-2</t>
-  </si>
-  <si>
     <t>2.2.2.1/24</t>
   </si>
   <si>
@@ -325,15 +325,6 @@
   </si>
   <si>
     <t>4.4.4.1/24</t>
-  </si>
-  <si>
-    <t>eigrp</t>
-  </si>
-  <si>
-    <t>10.2.1.1/30</t>
-  </si>
-  <si>
-    <t>10.2.2.1/30</t>
   </si>
   <si>
     <t>static</t>
@@ -719,7 +710,7 @@
     </row>
     <row r="2" hidden="false">
       <c r="A2" t="n" s="3">
-        <v>42858.0</v>
+        <v>42870.0</v>
       </c>
       <c r="B2" t="s" s="5">
         <v>72</v>
@@ -754,7 +745,9 @@
       <c r="L2" t="n" s="5">
         <v>100.0</v>
       </c>
-      <c r="M2" s="5"/>
+      <c r="M2" t="s" s="5">
+        <v>82</v>
+      </c>
       <c r="N2" t="s" s="5">
         <v>82</v>
       </c>
@@ -792,36 +785,36 @@
         <v>91</v>
       </c>
       <c r="Z2" t="s" s="5">
+        <v>85</v>
+      </c>
+      <c r="AA2" t="s" s="5">
         <v>92</v>
-      </c>
-      <c r="AA2" t="s" s="5">
-        <v>91</v>
       </c>
       <c r="AB2" t="s" s="5">
         <v>93</v>
       </c>
       <c r="AC2" t="s" s="5">
+        <v>92</v>
+      </c>
+      <c r="AD2" t="s" s="5">
         <v>94</v>
       </c>
-      <c r="AD2" t="s" s="5">
+      <c r="AE2" t="s" s="5">
+        <v>92</v>
+      </c>
+      <c r="AF2" t="s" s="5">
         <v>95</v>
       </c>
-      <c r="AE2" t="s" s="5">
-        <v>94</v>
-      </c>
-      <c r="AF2" s="5"/>
       <c r="AG2" t="s" s="5">
         <v>96</v>
       </c>
       <c r="AH2" t="n" s="5">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="AI2" t="s" s="5">
         <v>97</v>
       </c>
-      <c r="AJ2" t="n" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="AJ2" s="5"/>
       <c r="AK2" t="n" s="5">
         <v>2110.0</v>
       </c>
@@ -831,29 +824,27 @@
       <c r="AM2" t="s" s="5">
         <v>99</v>
       </c>
-      <c r="AN2" t="s" s="5">
-        <v>100</v>
-      </c>
+      <c r="AN2" s="5"/>
       <c r="AO2" t="s" s="5">
         <v>91</v>
       </c>
       <c r="AP2" t="s" s="5">
+        <v>100</v>
+      </c>
+      <c r="AQ2" t="s" s="5">
         <v>92</v>
-      </c>
-      <c r="AQ2" t="s" s="5">
-        <v>94</v>
       </c>
       <c r="AR2" t="s" s="5">
         <v>101</v>
       </c>
       <c r="AS2" t="s" s="5">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AT2" t="s" s="5">
         <v>102</v>
       </c>
       <c r="AU2" t="s" s="5">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AV2" t="s" s="5">
         <v>103</v>
@@ -863,45 +854,39 @@
       </c>
       <c r="AX2" s="5"/>
       <c r="AY2" s="5"/>
-      <c r="AZ2" t="n" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="AZ2" s="5"/>
       <c r="BA2" t="n" s="5">
         <v>2111.0</v>
       </c>
-      <c r="BB2" t="s" s="5">
-        <v>105</v>
-      </c>
-      <c r="BC2" t="s" s="5">
-        <v>106</v>
-      </c>
+      <c r="BB2" s="5"/>
+      <c r="BC2" s="5"/>
       <c r="BD2" s="5"/>
       <c r="BE2" t="s" s="5">
         <v>91</v>
       </c>
       <c r="BF2" t="s" s="5">
+        <v>100</v>
+      </c>
+      <c r="BG2" t="s" s="5">
         <v>92</v>
-      </c>
-      <c r="BG2" t="s" s="5">
-        <v>94</v>
       </c>
       <c r="BH2" t="s" s="5">
         <v>101</v>
       </c>
       <c r="BI2" t="s" s="5">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="BJ2" t="s" s="5">
         <v>102</v>
       </c>
       <c r="BK2" t="s" s="5">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="BL2" t="s" s="5">
         <v>103</v>
       </c>
       <c r="BM2" t="s" s="5">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="BN2" s="5"/>
       <c r="BO2" s="5"/>

</xml_diff>